<commit_message>
after plotting the compr depth vs bouguer
</commit_message>
<xml_diff>
--- a/inv/Inv-Brief-20iter.xlsx
+++ b/inv/Inv-Brief-20iter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sina/Desktop/RFCAN/rfcan/inv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60DE33DA-B30C-7D42-8369-40344927CB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6980DD4D-54F0-1149-849C-8EB4BE81C9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2300" yWindow="500" windowWidth="35960" windowHeight="28300" xr2:uid="{5CEBB106-7F0F-544B-A2D0-333EF0922D30}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="134">
   <si>
     <t>station</t>
   </si>
@@ -457,6 +457,9 @@
   </si>
   <si>
     <t>SelectedVpVs</t>
+  </si>
+  <si>
+    <t>Superior Province</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1021,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1077,6 +1080,7 @@
     <xf numFmtId="1" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1842,7 +1846,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="7194550" y="9207500"/>
-              <a:ext cx="10229850" cy="2743200"/>
+              <a:ext cx="11880850" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2192,10 +2196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63138A22-43F4-1F44-BF9B-6A57854762C5}">
-  <dimension ref="A1:BU65"/>
+  <dimension ref="A1:BU66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="F66" sqref="F66:J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12013,6 +12017,15 @@
       </c>
     </row>
     <row r="55" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B55" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>2.6</v>
+      </c>
       <c r="F55" s="13" t="s">
         <v>115</v>
       </c>
@@ -12201,6 +12214,23 @@
       <c r="P65" s="35"/>
       <c r="Q65" s="5"/>
     </row>
+    <row r="66" spans="6:17" x14ac:dyDescent="0.2">
+      <c r="F66" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="G66" s="36">
+        <v>41223</v>
+      </c>
+      <c r="H66" s="36">
+        <v>6404</v>
+      </c>
+      <c r="I66" s="36">
+        <v>3348</v>
+      </c>
+      <c r="J66" s="36">
+        <v>1.91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>